<commit_message>
sma supported on daily & minutely
</commit_message>
<xml_diff>
--- a/documentation/indicators.xlsx
+++ b/documentation/indicators.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,6 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\github\sbCryptoWork\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE9F36C-4D64-46D0-B4A6-03FFD299D83E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="12" windowWidth="20952" windowHeight="9720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="47">
   <si>
     <t>No</t>
   </si>
@@ -157,13 +158,16 @@
   </si>
   <si>
     <t>=not yet</t>
+  </si>
+  <si>
+    <t>DHM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +210,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -222,7 +232,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
@@ -351,7 +361,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -403,8 +413,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -908,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -919,7 +930,7 @@
     <col min="3" max="3" width="54.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.5546875" style="1" bestFit="1"/>
     <col min="5" max="5" width="19.88671875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" style="1" customWidth="1"/>
     <col min="7" max="9" width="9.109375" style="1"/>
     <col min="10" max="10" width="11.44140625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9.109375" style="1"/>
@@ -959,8 +970,8 @@
         <v>7</v>
       </c>
       <c r="F4" s="20"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="26" t="s">
+      <c r="H4" s="26"/>
+      <c r="I4" s="25" t="s">
         <v>44</v>
       </c>
     </row>
@@ -979,7 +990,7 @@
       </c>
       <c r="F5" s="20"/>
       <c r="H5" s="11"/>
-      <c r="I5" s="26" t="s">
+      <c r="I5" s="25" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1156,7 +1167,9 @@
       <c r="E21" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="11"/>
+      <c r="F21" s="27" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" s="8">
@@ -1171,7 +1184,7 @@
       <c r="E22" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="11"/>
+      <c r="F22" s="26"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" s="8">
@@ -1186,7 +1199,7 @@
       <c r="E23" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="11"/>
+      <c r="F23" s="26"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24" s="8">
@@ -1201,7 +1214,7 @@
       <c r="E24" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="11"/>
+      <c r="F24" s="26"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" s="8">
@@ -1216,7 +1229,7 @@
       <c r="E25" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F25" s="11"/>
+      <c r="F25" s="26"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" s="8">
@@ -1231,7 +1244,7 @@
       <c r="E26" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F26" s="11"/>
+      <c r="F26" s="26"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27" s="8">

</xml_diff>